<commit_message>
Committing additional test cases for phs002371
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs000720_Sex-Female_Race-White_diseasephs-Relapse.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs000720_Sex-Female_Race-White_diseasephs-Relapse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\03-31-25\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\04-29-25\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91742114-4BCC-4D95-A38F-2B507285D012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C6FB70-96AC-4100-8A84-218B8BF428D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -261,9 +261,8 @@
     fd.file_access AS "File Access",
     std.dbgap_accession AS "Study ID",
     prt.participant_id AS "Participant ID",
-    smp.sample_id AS "Sample ID",
-    fd.file_source AS "File Source"
-FROM 
+    smp.sample_id AS "Sample ID"
+  FROM 
     df_study std
 LEFT JOIN df_participant prt ON std.id = prt."study.id"
 LEFT JOIN df_sample smp ON prt.id = smp."participant.id"

</xml_diff>

<commit_message>
CCDI - Add GUID helper method and handle adding and sorting GUID column for Files tab for related studies, plus query fixes
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs000720_Sex-Female_Race-White_diseasephs-Relapse.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs000720_Sex-Female_Race-White_diseasephs-Relapse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75E5A50-97F2-FE42-BE9C-03F32EFB7CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DDAA87-5C35-274C-ADF6-3A9E719C77FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="30860" windowHeight="19240" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -481,8 +481,8 @@
   END                                AS "File Size",
   ef.file_access                     AS "File Access",
   'phs000720'                        AS "Study ID",
-  '[' || prt.participant_id || ']'   AS "Participant ID",
-  '[' || smp.sample_id || ']'        AS "Sample ID"
+  prt.participant_id   AS "Participant ID",
+  smp.sample_id        AS "Sample ID"
 FROM eligible_files ef
 JOIN df_sample smp
   ON smp.id = ef.sample_row_id
@@ -496,9 +496,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -565,14 +572,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -901,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -969,7 +979,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="2"/>
@@ -982,7 +992,7 @@
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>